<commit_message>
Leadership task modified to use PK
</commit_message>
<xml_diff>
--- a/DynamoDBSQL/dynamosql/src/assets/csv/leaderboard.xlsx
+++ b/DynamoDBSQL/dynamosql/src/assets/csv/leaderboard.xlsx
@@ -44,18 +44,12 @@
     <t>Ian Porter</t>
   </si>
   <si>
-    <t> USA</t>
-  </si>
-  <si>
     <t>JJoNak</t>
   </si>
   <si>
     <t>Bang Seong-hyun</t>
   </si>
   <si>
-    <t> KOR</t>
-  </si>
-  <si>
     <t>Seagull</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
     <t>Félix Lengyel</t>
   </si>
   <si>
-    <t> CAN</t>
-  </si>
-  <si>
     <t>Park Se-jun</t>
   </si>
   <si>
@@ -86,9 +77,6 @@
     <t>Dennis Johnsen</t>
   </si>
   <si>
-    <t> DNK</t>
-  </si>
-  <si>
     <t>Dardoch</t>
   </si>
   <si>
@@ -134,18 +122,12 @@
     <t>Emil Christensen</t>
   </si>
   <si>
-    <t> SWE</t>
-  </si>
-  <si>
     <t>Ferrari_430</t>
   </si>
   <si>
     <t>Luo Feichi</t>
   </si>
   <si>
-    <t> CHN</t>
-  </si>
-  <si>
     <t>Jaedong</t>
   </si>
   <si>
@@ -164,9 +146,6 @@
     <t>Danylo Ishutin</t>
   </si>
   <si>
-    <t> UKR</t>
-  </si>
-  <si>
     <t>MaDFroG</t>
   </si>
   <si>
@@ -177,6 +156,27 @@
   </si>
   <si>
     <t>country</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>KOR</t>
+  </si>
+  <si>
+    <t>CAN</t>
+  </si>
+  <si>
+    <t>DNK</t>
+  </si>
+  <si>
+    <t>SWE</t>
+  </si>
+  <si>
+    <t>CHN</t>
+  </si>
+  <si>
+    <t>UKR</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,10 +520,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -544,7 +544,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2">
         <v>514</v>
@@ -559,13 +559,13 @@
         <v>28112</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="E3" s="2">
         <v>674</v>
@@ -580,13 +580,13 @@
         <v>28113</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="E4" s="2">
         <v>315</v>
@@ -601,13 +601,13 @@
         <v>28114</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2">
         <v>227</v>
@@ -622,13 +622,13 @@
         <v>28115</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="E6" s="2">
         <v>462</v>
@@ -643,13 +643,13 @@
         <v>28116</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="E7" s="2">
         <v>728</v>
@@ -664,13 +664,13 @@
         <v>28117</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="E8" s="2">
         <v>457</v>
@@ -685,13 +685,13 @@
         <v>28118</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="E9" s="2">
         <v>975</v>
@@ -706,13 +706,13 @@
         <v>28119</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="E10" s="2">
         <v>350</v>
@@ -727,13 +727,13 @@
         <v>28120</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="E11" s="2">
         <v>451</v>
@@ -748,13 +748,13 @@
         <v>28121</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="E12" s="2">
         <v>205</v>
@@ -769,13 +769,13 @@
         <v>28122</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="E13" s="2">
         <v>777</v>
@@ -790,13 +790,13 @@
         <v>28123</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="E14" s="2">
         <v>321</v>
@@ -811,13 +811,13 @@
         <v>28124</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="E15" s="2">
         <v>677</v>
@@ -832,13 +832,13 @@
         <v>28125</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="E16" s="2">
         <v>432</v>
@@ -853,13 +853,13 @@
         <v>28126</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E17" s="2">
         <v>685</v>
@@ -874,13 +874,13 @@
         <v>28127</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="E18" s="2">
         <v>458</v>
@@ -895,13 +895,13 @@
         <v>28128</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="E19" s="2">
         <v>534</v>
@@ -916,13 +916,13 @@
         <v>28129</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E20" s="2">
         <v>762</v>
@@ -937,13 +937,13 @@
         <v>28130</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" t="s">
         <v>48</v>
-      </c>
-      <c r="D21" t="s">
-        <v>36</v>
       </c>
       <c r="E21" s="2">
         <v>601</v>

</xml_diff>